<commit_message>
SON24 new content: Charts and tables: IN23: Highest qualification: Review mark-ups
</commit_message>
<xml_diff>
--- a/son/content/intermediate_outcomes/routes_into_work_(16_to_29_years)/highest_qualification/2.0/IN23-2.0-highest-qualification--by-SEB--table-format.xlsx
+++ b/son/content/intermediate_outcomes/routes_into_work_(16_to_29_years)/highest_qualification/2.0/IN23-2.0-highest-qualification--by-SEB--table-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\intermediate_outcomes\routes_into_work_(16_to_29_years)\highest_qualification\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02971437-1F99-4D59-8F3B-29DEE6F29F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87C1060-AB04-40D0-8D5C-C151DB27C33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{FAB25B7A-4F11-420B-91E9-BB4ABC51D39A}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3652" uniqueCount="113">
   <si>
     <t>ind_code</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Socio-economic background</t>
-  </si>
-  <si>
-    <t>All backgrounds</t>
   </si>
 </sst>
 </file>
@@ -6744,7 +6741,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F276F431-A7F3-4DCB-A718-41AB23F9C8C8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Socio-economic background">
-  <location ref="A5:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <location ref="A5:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -6766,7 +6763,7 @@
         <item x="2"/>
         <item x="1"/>
         <item x="0"/>
-        <item n="All backgrounds" x="5"/>
+        <item n="All backgrounds" h="1" x="5"/>
         <item h="1" x="6"/>
         <item t="default"/>
       </items>
@@ -6841,7 +6838,7 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
@@ -6856,9 +6853,6 @@
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -7221,10 +7215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C030DE3-7094-4EDA-A1C4-21FA542C37CE}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -7421,29 +7415,6 @@
         <v>7.3597920900206004</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="3">
-        <v>9.4737232975250105</v>
-      </c>
-      <c r="C12" s="3">
-        <v>13.320688489425599</v>
-      </c>
-      <c r="D12" s="3">
-        <v>21.759003186573601</v>
-      </c>
-      <c r="E12" s="3">
-        <v>5.9729801889345602</v>
-      </c>
-      <c r="F12" s="3">
-        <v>33.334479965227402</v>
-      </c>
-      <c r="G12" s="3">
-        <v>15.9526187401872</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>